<commit_message>
ADDED ICONS ACROSS FORMS, ADDED TOOLTIPS ON AUDIT TRAIL
</commit_message>
<xml_diff>
--- a/teacher_records_full.xlsx
+++ b/teacher_records_full.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PROJECTS\CBCentra\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0E9310-7A98-4801-BA85-5EA4254B0157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="335">
   <si>
     <t>teacher_id_code</t>
   </si>
@@ -1018,68 +1024,14 @@
     <t>Teacher</t>
   </si>
   <si>
-    <t>1,292,096</t>
-  </si>
-  <si>
-    <t>1,260,937</t>
-  </si>
-  <si>
-    <t>535,101</t>
-  </si>
-  <si>
-    <t>1,243,880</t>
-  </si>
-  <si>
-    <t>1,128,159</t>
-  </si>
-  <si>
-    <t>1,056,602</t>
-  </si>
-  <si>
-    <t>1,487,803</t>
-  </si>
-  <si>
-    <t>598,181</t>
-  </si>
-  <si>
-    <t>1,447,626</t>
-  </si>
-  <si>
-    <t>463,831</t>
-  </si>
-  <si>
-    <t>624,128</t>
-  </si>
-  <si>
-    <t>864,175</t>
-  </si>
-  <si>
-    <t>1,291,269</t>
-  </si>
-  <si>
-    <t>699,530</t>
-  </si>
-  <si>
-    <t>1,381,883</t>
-  </si>
-  <si>
-    <t>533,162</t>
-  </si>
-  <si>
-    <t>496,684</t>
-  </si>
-  <si>
-    <t>727,022</t>
-  </si>
-  <si>
-    <t>Masala Senior Secondary</t>
+    <t>Heaven is my Home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1104,27 +1056,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1133,22 +1070,28 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1186,7 +1129,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1220,6 +1163,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1254,9 +1198,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1429,14 +1374,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1513,7 +1485,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1583,14 +1555,14 @@
       <c r="W2" t="s">
         <v>326</v>
       </c>
-      <c r="X2" t="s">
+      <c r="X2">
+        <v>800000</v>
+      </c>
+      <c r="Y2" t="s">
         <v>334</v>
       </c>
-      <c r="Y2" t="s">
-        <v>352</v>
-      </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1660,14 +1632,14 @@
       <c r="W3" t="s">
         <v>327</v>
       </c>
-      <c r="X3" t="s">
-        <v>335</v>
+      <c r="X3">
+        <v>800000</v>
       </c>
       <c r="Y3" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -1737,14 +1709,14 @@
       <c r="W4" t="s">
         <v>328</v>
       </c>
-      <c r="X4" t="s">
-        <v>336</v>
+      <c r="X4">
+        <v>800000</v>
       </c>
       <c r="Y4" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1814,14 +1786,14 @@
       <c r="W5" t="s">
         <v>329</v>
       </c>
-      <c r="X5" t="s">
-        <v>337</v>
+      <c r="X5">
+        <v>800000</v>
       </c>
       <c r="Y5" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1891,14 +1863,14 @@
       <c r="W6" t="s">
         <v>330</v>
       </c>
-      <c r="X6" t="s">
-        <v>338</v>
+      <c r="X6">
+        <v>800000</v>
       </c>
       <c r="Y6" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -1968,14 +1940,14 @@
       <c r="W7" t="s">
         <v>330</v>
       </c>
-      <c r="X7" t="s">
-        <v>339</v>
+      <c r="X7">
+        <v>800000</v>
       </c>
       <c r="Y7" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -2045,14 +2017,14 @@
       <c r="W8" t="s">
         <v>331</v>
       </c>
-      <c r="X8" t="s">
-        <v>340</v>
+      <c r="X8">
+        <v>800000</v>
       </c>
       <c r="Y8" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2122,14 +2094,14 @@
       <c r="W9" t="s">
         <v>326</v>
       </c>
-      <c r="X9" t="s">
-        <v>341</v>
+      <c r="X9">
+        <v>800000</v>
       </c>
       <c r="Y9" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2199,14 +2171,14 @@
       <c r="W10" t="s">
         <v>332</v>
       </c>
-      <c r="X10" t="s">
-        <v>342</v>
+      <c r="X10">
+        <v>800000</v>
       </c>
       <c r="Y10" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2276,14 +2248,14 @@
       <c r="W11" t="s">
         <v>329</v>
       </c>
-      <c r="X11" t="s">
-        <v>343</v>
+      <c r="X11">
+        <v>800000</v>
       </c>
       <c r="Y11" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -2353,14 +2325,14 @@
       <c r="W12" t="s">
         <v>326</v>
       </c>
-      <c r="X12" t="s">
-        <v>344</v>
+      <c r="X12">
+        <v>800000</v>
       </c>
       <c r="Y12" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -2430,14 +2402,14 @@
       <c r="W13" t="s">
         <v>327</v>
       </c>
-      <c r="X13" t="s">
-        <v>345</v>
+      <c r="X13">
+        <v>800000</v>
       </c>
       <c r="Y13" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2507,14 +2479,14 @@
       <c r="W14" t="s">
         <v>333</v>
       </c>
-      <c r="X14" t="s">
-        <v>346</v>
+      <c r="X14">
+        <v>800000</v>
       </c>
       <c r="Y14" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -2584,14 +2556,14 @@
       <c r="W15" t="s">
         <v>330</v>
       </c>
-      <c r="X15" t="s">
-        <v>347</v>
+      <c r="X15">
+        <v>800000</v>
       </c>
       <c r="Y15" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>39</v>
       </c>
@@ -2661,14 +2633,14 @@
       <c r="W16" t="s">
         <v>328</v>
       </c>
-      <c r="X16" t="s">
-        <v>348</v>
+      <c r="X16">
+        <v>800000</v>
       </c>
       <c r="Y16" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>40</v>
       </c>
@@ -2738,14 +2710,14 @@
       <c r="W17" t="s">
         <v>329</v>
       </c>
-      <c r="X17" t="s">
-        <v>349</v>
+      <c r="X17">
+        <v>800000</v>
       </c>
       <c r="Y17" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -2815,14 +2787,14 @@
       <c r="W18" t="s">
         <v>327</v>
       </c>
-      <c r="X18" t="s">
-        <v>350</v>
+      <c r="X18">
+        <v>800000</v>
       </c>
       <c r="Y18" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -2892,11 +2864,11 @@
       <c r="W19" t="s">
         <v>332</v>
       </c>
-      <c r="X19" t="s">
-        <v>351</v>
+      <c r="X19">
+        <v>800000</v>
       </c>
       <c r="Y19" t="s">
-        <v>352</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>